<commit_message>
fixed LIB party straight ticket
</commit_message>
<xml_diff>
--- a/MI_Chippewa/MI_Chippewa_GE20_cleaned.xlsx
+++ b/MI_Chippewa/MI_Chippewa_GE20_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\MI_Chippewa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF8B960-4A2B-4E97-8B30-6E1A0D7FC678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAAFBF3-3073-4911-8A02-79BC82E84B10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="370" windowWidth="30880" windowHeight="18760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17520" yWindow="3380" windowWidth="20270" windowHeight="13880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total_reg_and_cast" sheetId="2" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>Republican Party - REP</t>
   </si>
   <si>
-    <t>Libertarian Party -LIB</t>
-  </si>
-  <si>
     <t>U.S. Taxpayers Party - UST</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>John N. Damoose - REP</t>
+  </si>
+  <si>
+    <t>Libertarian Party - LIB</t>
   </si>
 </sst>
 </file>
@@ -840,20 +840,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2FF416-A3A0-4C25-94E4-19DAAAF79FB9}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -867,19 +867,19 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1510,25 +1510,25 @@
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2054,22 +2054,22 @@
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2536,16 +2536,16 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2880,7 +2880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12538D38-9969-48EA-B070-6F1EB35D34F9}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -2896,13 +2896,13 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>